<commit_message>
Se actualiza lista de entradas y salidas.
</commit_message>
<xml_diff>
--- a/Diagramas/entradas y salidas.xlsx
+++ b/Diagramas/entradas y salidas.xlsx
@@ -16,9 +16,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>P40</t>
+  </si>
+  <si>
+    <t>P00</t>
+  </si>
+  <si>
+    <t>P01</t>
+  </si>
+  <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
+    <t>P05</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>P07</t>
+  </si>
+  <si>
+    <t>P08</t>
+  </si>
+  <si>
+    <t>P09</t>
+  </si>
+  <si>
+    <t>P0A</t>
+  </si>
+  <si>
+    <t>P0B</t>
+  </si>
+  <si>
+    <t>P0C</t>
+  </si>
+  <si>
+    <t>P0D</t>
+  </si>
+  <si>
+    <t>P0E</t>
+  </si>
+  <si>
+    <t>P0F</t>
+  </si>
+  <si>
+    <t>P11</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P14</t>
+  </si>
+  <si>
+    <t>P15</t>
+  </si>
+  <si>
+    <t>P16</t>
+  </si>
+  <si>
+    <t>P17</t>
+  </si>
+  <si>
+    <t>P41</t>
+  </si>
+  <si>
+    <t>P42</t>
+  </si>
+  <si>
+    <t>P43</t>
+  </si>
+  <si>
+    <t>P44</t>
+  </si>
+  <si>
+    <t>P45</t>
+  </si>
+  <si>
+    <t>P46</t>
+  </si>
+  <si>
+    <t>P47</t>
+  </si>
+  <si>
+    <t>P48</t>
+  </si>
+  <si>
+    <t>P49</t>
+  </si>
+  <si>
+    <t>P4A</t>
+  </si>
+  <si>
+    <t>P4B</t>
+  </si>
+  <si>
+    <t>P4C</t>
+  </si>
+  <si>
+    <t>P4D</t>
+  </si>
+  <si>
+    <t>P4E</t>
+  </si>
+  <si>
+    <t>P4F</t>
+  </si>
+  <si>
+    <t>Torreta</t>
+  </si>
+  <si>
+    <t>Volquete</t>
+  </si>
+  <si>
+    <t>Bajar maquina</t>
+  </si>
+  <si>
+    <t>GiroDerecha</t>
+  </si>
+  <si>
+    <t>GiroIzquierda</t>
+  </si>
+  <si>
+    <t>Desague</t>
+  </si>
+  <si>
+    <t>AguaFria</t>
+  </si>
+  <si>
+    <t>AguaCaliente</t>
+  </si>
+  <si>
+    <t>Vapor</t>
+  </si>
+  <si>
+    <t>Programa lav-tupesa</t>
+  </si>
+  <si>
+    <t>Lista de entrada y salidas del PLC</t>
+  </si>
+  <si>
+    <t>CuentaLitros</t>
+  </si>
+  <si>
+    <t>MaquinaArriba</t>
+  </si>
+  <si>
+    <t>ParoEmergencia (NC)</t>
+  </si>
+  <si>
+    <t>EnjuagueQuimicos</t>
+  </si>
+  <si>
+    <t>IntroducirQuimicos</t>
+  </si>
+  <si>
+    <t>SegurosPuerta</t>
+  </si>
+  <si>
+    <t>VelocidadCentrifuga</t>
   </si>
 </sst>
 </file>
@@ -34,15 +202,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -50,12 +236,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,21 +573,280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F3"/>
+  <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="E7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="E9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="E10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="E13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="E16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="E17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="E18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="E19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se libera version 1.04 de plc y 1.04 de hmi. * Calentamiento con control proporcional.
</commit_message>
<xml_diff>
--- a/Diagramas/entradas y salidas.xlsx
+++ b/Diagramas/entradas y salidas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>P40</t>
   </si>
@@ -187,6 +187,21 @@
   </si>
   <si>
     <t>VelocidadCentrifuga</t>
+  </si>
+  <si>
+    <t>FrenoTombola</t>
+  </si>
+  <si>
+    <t>MaquinaHorizontal</t>
+  </si>
+  <si>
+    <t>MaquinaAbajo</t>
+  </si>
+  <si>
+    <t>PuertaCerrada</t>
+  </si>
+  <si>
+    <t>PuertaAbierta</t>
   </si>
 </sst>
 </file>
@@ -576,7 +591,7 @@
   <dimension ref="B1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +667,9 @@
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
@@ -664,7 +681,9 @@
       <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
@@ -676,7 +695,9 @@
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="E9" s="5" t="s">
         <v>28</v>
       </c>
@@ -688,7 +709,9 @@
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
@@ -776,7 +799,9 @@
       <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">

</xml_diff>

<commit_message>
Se libera version 1.05 de PLC y HMI. * Se agrega paso centrifugado (#7)
</commit_message>
<xml_diff>
--- a/Diagramas/entradas y salidas.xlsx
+++ b/Diagramas/entradas y salidas.xlsx
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +787,7 @@
       <c r="E16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se libera version 1.06 de PLC y 1.06 de HMI.
</commit_message>
<xml_diff>
--- a/Diagramas/entradas y salidas.xlsx
+++ b/Diagramas/entradas y salidas.xlsx
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se agrega checklist de entrega y lista de parametros
</commit_message>
<xml_diff>
--- a/Diagramas/entradas y salidas.xlsx
+++ b/Diagramas/entradas y salidas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>P40</t>
   </si>
@@ -202,16 +202,52 @@
   </si>
   <si>
     <t>PuertaAbierta</t>
+  </si>
+  <si>
+    <t>CH0</t>
+  </si>
+  <si>
+    <t>CH1</t>
+  </si>
+  <si>
+    <t>CH2</t>
+  </si>
+  <si>
+    <t>CH3</t>
+  </si>
+  <si>
+    <t>PT100</t>
+  </si>
+  <si>
+    <t>Modulo analogo RTD</t>
+  </si>
+  <si>
+    <t>Modulo analogo</t>
+  </si>
+  <si>
+    <t>Generador Ozono</t>
+  </si>
+  <si>
+    <t>GeneradorOzono</t>
+  </si>
+  <si>
+    <t>QuemadorOzono</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -266,11 +302,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -287,6 +334,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F26"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,272 +661,350 @@
     <col min="7" max="7" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="E11" s="5" t="s">
+      <c r="C12" s="3"/>
+      <c r="E12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="E12" s="4" t="s">
+      <c r="C13" s="2"/>
+      <c r="E13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="E13" s="5" t="s">
+      <c r="C14" s="3"/>
+      <c r="E14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="E14" s="4" t="s">
+      <c r="C15" s="2"/>
+      <c r="E15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="E15" s="5" t="s">
+      <c r="C16" s="3"/>
+      <c r="E16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="E16" s="4" t="s">
+      <c r="C17" s="2"/>
+      <c r="E17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="E17" s="5" t="s">
+      <c r="C18" s="3"/>
+      <c r="E18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="E18" s="4" t="s">
+      <c r="C19" s="2"/>
+      <c r="E19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="F19" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="E19" s="5" t="s">
+      <c r="C20" s="3"/>
+      <c r="E20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="F20" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="E38" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C39" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B36:F36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>

</xml_diff>